<commit_message>
Updated excel import service with better validations
</commit_message>
<xml_diff>
--- a/ApplicationRecords_Import_Template.xlsx
+++ b/ApplicationRecords_Import_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\FullStackProject\ApplicationTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4757DF04-0071-4484-BCFF-F44E88A8D0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456525B2-A7DF-4F36-B214-97DF6716D93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="5085" windowWidth="28800" windowHeight="15435" xr2:uid="{0DC61EF3-0AB4-4D72-BBD1-F2775F03C231}"/>
+    <workbookView xWindow="-38520" yWindow="-60" windowWidth="38640" windowHeight="21240" xr2:uid="{0DC61EF3-0AB4-4D72-BBD1-F2775F03C231}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E3"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +426,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">

</xml_diff>